<commit_message>
Server recebe + pedidos
</commit_message>
<xml_diff>
--- a/input/Nomes.xlsx
+++ b/input/Nomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35193\Desktop\bolsa\bolsa_meu\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A50D41A-5B25-48FE-8F2B-B8F2CDF7CA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70F40A-EFF4-4BC1-8D95-69D68727F154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Técnicos" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Zé 1</t>
   </si>
   <si>
-    <t>Zé 2</t>
-  </si>
-  <si>
     <t>Zé 3</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Projeto 17</t>
+  </si>
+  <si>
+    <t>Manel 2</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63805B2B-5AD1-4D6A-B2D6-762A66709158}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
@@ -592,10 +592,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -699,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -739,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expreiências sobre estados de análise
</commit_message>
<xml_diff>
--- a/input/Nomes.xlsx
+++ b/input/Nomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35193\Desktop\bolsa\bolsa_meu\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70F40A-EFF4-4BC1-8D95-69D68727F154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB20CA7-D8EF-419C-B235-B037540C13D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Técnicos" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
     <t>Zé 1</t>
   </si>
   <si>
-    <t>Zé 3</t>
-  </si>
-  <si>
     <t>Zé 4</t>
   </si>
   <si>
@@ -76,12 +73,6 @@
     <t>Projeto nome</t>
   </si>
   <si>
-    <t>Projeto 0</t>
-  </si>
-  <si>
-    <t>Projeto 1</t>
-  </si>
-  <si>
     <t>Projeto 2</t>
   </si>
   <si>
@@ -130,7 +121,16 @@
     <t>Projeto 17</t>
   </si>
   <si>
-    <t>Manel 2</t>
+    <t>Zé 2</t>
+  </si>
+  <si>
+    <t>Manel 3</t>
+  </si>
+  <si>
+    <t>ANI1</t>
+  </si>
+  <si>
+    <t>Ani2</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -584,18 +584,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63805B2B-5AD1-4D6A-B2D6-762A66709158}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -699,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -739,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Começa a responder info de projetos
Falta responder info de pedidos, e ajustar frontend a receber info
</commit_message>
<xml_diff>
--- a/input/Nomes.xlsx
+++ b/input/Nomes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35193\Desktop\bolsa\bolsa_meu\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB20CA7-D8EF-419C-B235-B037540C13D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF93C431-F6D7-4568-8CC2-694B2D7C78D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Técnicos" sheetId="1" r:id="rId1"/>
@@ -127,10 +127,10 @@
     <t>Manel 3</t>
   </si>
   <si>
-    <t>ANI1</t>
-  </si>
-  <si>
-    <t>Ani2</t>
+    <t>ANI0</t>
+  </si>
+  <si>
+    <t>Ani1</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63805B2B-5AD1-4D6A-B2D6-762A66709158}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agora excel tem butões
</commit_message>
<xml_diff>
--- a/input/Nomes.xlsx
+++ b/input/Nomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\35193\Desktop\bolsa\bolsa_meu\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF93C431-F6D7-4568-8CC2-694B2D7C78D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D416D69-15D1-47F5-9E70-37E92E26F2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Técnicos" sheetId="1" r:id="rId1"/>
@@ -34,39 +34,6 @@
     <t>Técnico nome</t>
   </si>
   <si>
-    <t>Zé 0</t>
-  </si>
-  <si>
-    <t>Zé 1</t>
-  </si>
-  <si>
-    <t>Zé 4</t>
-  </si>
-  <si>
-    <t>Zé 5</t>
-  </si>
-  <si>
-    <t>Zé 6</t>
-  </si>
-  <si>
-    <t>Zé 7</t>
-  </si>
-  <si>
-    <t>Zé 8</t>
-  </si>
-  <si>
-    <t>Zé 9</t>
-  </si>
-  <si>
-    <t>Zé 10</t>
-  </si>
-  <si>
-    <t>Zé 11</t>
-  </si>
-  <si>
-    <t>Zé 12</t>
-  </si>
-  <si>
     <t>Projeto id</t>
   </si>
   <si>
@@ -121,16 +88,49 @@
     <t>Projeto 17</t>
   </si>
   <si>
-    <t>Zé 2</t>
-  </si>
-  <si>
-    <t>Manel 3</t>
-  </si>
-  <si>
-    <t>ANI0</t>
-  </si>
-  <si>
-    <t>Ani1</t>
+    <t>Técnico 0</t>
+  </si>
+  <si>
+    <t>Técnico 1</t>
+  </si>
+  <si>
+    <t>Técnico 2</t>
+  </si>
+  <si>
+    <t>Técnico 3</t>
+  </si>
+  <si>
+    <t>Técnico 4</t>
+  </si>
+  <si>
+    <t>Técnico 5</t>
+  </si>
+  <si>
+    <t>Técnico 6</t>
+  </si>
+  <si>
+    <t>Técnico 7</t>
+  </si>
+  <si>
+    <t>Técnico 8</t>
+  </si>
+  <si>
+    <t>Técnico 9</t>
+  </si>
+  <si>
+    <t>Técnico 10</t>
+  </si>
+  <si>
+    <t>Técnico 11</t>
+  </si>
+  <si>
+    <t>Técnico 12</t>
+  </si>
+  <si>
+    <t>Projeto 0</t>
+  </si>
+  <si>
+    <t>Projeto 1</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -483,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -547,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -563,7 +563,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -584,18 +584,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63805B2B-5AD1-4D6A-B2D6-762A66709158}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -619,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -667,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -691,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -699,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -715,7 +715,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -723,7 +723,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -731,7 +731,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -739,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>